<commit_message>
implemented the new TestEnvironment and TestNgTestClassTemplate framework
</commit_message>
<xml_diff>
--- a/src/test/resources/bluesource/dataProviders/TestAddNewDept.xlsx
+++ b/src/test/resources/bluesource/dataProviders/TestAddNewDept.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="18195" windowHeight="6975"/>
   </bookViews>
   <sheets>
-    <sheet name="TestAddNewTitle" sheetId="1" r:id="rId1"/>
+    <sheet name="TestAddNewDept" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -37,8 +37,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,6 +565,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -643,6 +648,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -677,6 +683,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -852,16 +859,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -872,7 +879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>

</xml_diff>